<commit_message>
ejercicio torres de hanoi en c++
</commit_message>
<xml_diff>
--- a/AlgoritmosBusquedasPorOrdenamiento/OrdenamientoPorBase/Ordenamiento por base.xlsx
+++ b/AlgoritmosBusquedasPorOrdenamiento/OrdenamientoPorBase/Ordenamiento por base.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>numero de datos</t>
   </si>
@@ -19,7 +19,10 @@
     <t>tiempo(miliseg)</t>
   </si>
   <si>
-    <t>10f(n/10)+n</t>
+    <t>n</t>
+  </si>
+  <si>
+    <t>nlog(n;10)</t>
   </si>
 </sst>
 </file>
@@ -52,7 +55,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -62,6 +65,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -163,11 +167,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1414615042"/>
-        <c:axId val="809640153"/>
+        <c:axId val="1820158656"/>
+        <c:axId val="1243856238"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1414615042"/>
+        <c:axId val="1820158656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -212,10 +216,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="809640153"/>
+        <c:crossAx val="1243856238"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="809640153"/>
+        <c:axId val="1243856238"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -284,7 +288,201 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1414615042"/>
+        <c:crossAx val="1820158656"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>nlog(n;10) frente a n</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Hoja 1'!$A$15:$A$25</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hoja 1'!$B$15:$B$25</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1390909328"/>
+        <c:axId val="657063693"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1390909328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="657063693"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="657063693"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>nlog(n;10)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1390909328"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -332,6 +530,31 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -641,8 +864,110 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:B18" si="1">(A15)*LOG(A15,10)</f>
+        <v>3.494850022</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="1"/>
+        <v>17.64136889</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="1"/>
+        <v>26.02059991</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="B19" s="3">
+        <f>(A15:A25)*LOG(A15:A25,10)</f>
+        <v>34.94850022</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="B20" s="3">
+        <f>(A15:A25)*LOG(A15:A25,10)</f>
+        <v>44.31363764</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
+        <v>35.0</v>
+      </c>
+      <c r="B21" s="3">
+        <f>(A15:A25)*LOG(A15:A25,10)</f>
+        <v>54.04238155</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="B22" s="3">
+        <f>(A15:A25)*LOG(A15:A25,10)</f>
+        <v>64.08239965</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2">
+        <v>45.0</v>
+      </c>
+      <c r="B23" s="3">
+        <f>(A15:A25)*LOG(A15:A25,10)</f>
+        <v>74.39456312</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="B24" s="3">
+        <f>(A15:A25)*LOG(A15:A25,10)</f>
+        <v>84.94850022</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="B25" s="3">
+        <f>(A15:A25)*LOG(A15:A25,10)</f>
+        <v>95.71994792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>